<commit_message>
Toimivat pakkaus- ja purkuoperaatiot.
Toimivat pakkaus- ja purkuoperaatiot (tosin Javan standardikalusto vielä
käytössä).
</commit_message>
<xml_diff>
--- a/Dokumentit/Tuntikirjanpito.xlsx
+++ b/Dokumentit/Tuntikirjanpito.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="16275" windowHeight="9780"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="16275" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Tietorakenteiden ja Algoritmien harjoitustyö, periodi II</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Luetun tiedoston Huffman-koodien tulostus System.Outiin ja puun toiminnan varmentamista Eclipsen debuggerilla. Junit testien aloittamista, JavaDocien kirjoittamista.</t>
+  </si>
+  <si>
+    <t>Kohdetiedoston "dummy" kirjoitus (Huffman-koodit dumppautuu nyt kohdetiedostoon). Ennen kaikkea kuitenkin refaktorointia ja koodin siistimistä.</t>
+  </si>
+  <si>
+    <t>Kohdetiedoston "oikea" kirjoitus. Sanastoa ei vielä kirjoiteta tiedoston alkuun joten purkaminen ei onnistu.</t>
+  </si>
+  <si>
+    <t>Sanaston kirjoitus tiedoston alkuun. Purkualgoritmin aloitus.</t>
+  </si>
+  <si>
+    <t>Purkualgoritmin debuggausta. Purkualgoritmi mahdollisesti toimiikin jo oikein mutta Huffman-koodin pakkaus tavujen biteiksi lienee buginen. Nyt sekä pakkaus että purku toimii melkein: purussa vielä bugi joka tuottaa epämääräisiä virheitä striimin sekaan. Ongelma liittyy Huffman-koodiin joka luetaan kahdessa lohkossa levyltä (todiste: kun lohkokoko &gt; pakatun tiedoston koko, ongelma häviää).</t>
   </si>
 </sst>
 </file>
@@ -493,7 +505,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>41218</v>
       </c>
@@ -595,25 +607,49 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>41222</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>41223</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>41224</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>41225</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -661,7 +697,7 @@
       </c>
       <c r="B24" s="9">
         <f>SUM(B6:B23)</f>
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C24" s="8"/>
     </row>

</xml_diff>

<commit_message>
- Oma Hajautustaulukko-toteutus - Yksikkötestauksen laajuutta parannettu huomattavasti (Huffman-puulle puuttuu yksikkötestit vielä). - Päivitetyt JavaDocit - Testidata lisätty GitHubiin - Päivitetty tuntikirjanpito
</commit_message>
<xml_diff>
--- a/Dokumentit/Tuntikirjanpito.xlsx
+++ b/Dokumentit/Tuntikirjanpito.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Tietorakenteiden ja Algoritmien harjoitustyö, periodi II</t>
   </si>
@@ -66,7 +66,14 @@
     <t>Sanaston kirjoitus tiedoston alkuun. Purkualgoritmin aloitus.</t>
   </si>
   <si>
-    <t>Purkualgoritmin debuggausta. Purkualgoritmi mahdollisesti toimiikin jo oikein mutta Huffman-koodin pakkaus tavujen biteiksi lienee buginen. Nyt sekä pakkaus että purku toimii melkein: purussa vielä bugi joka tuottaa epämääräisiä virheitä striimin sekaan. Ongelma liittyy Huffman-koodiin joka luetaan kahdessa lohkossa levyltä (todiste: kun lohkokoko &gt; pakatun tiedoston koko, ongelma häviää).</t>
+    <t>Purkualgoritmin koodausta, debuggausta. Purkualgoritmi mahdollisesti toimiikin jo oikein mutta Huffman-koodin pakkaus tavujen biteiksi lienee buginen. Nyt sekä pakkaus että purku toimii melkein: purussa vielä bugi joka tuottaa epämääräisiä virheitä striimin sekaan. Ongelma liittyy Huffman-koodiin joka luetaan kahdessa lohkossa levyltä (todiste: kun lohkokoko &gt;= pakatun tiedoston koko, ongelma häviää).</t>
+  </si>
+  <si>
+    <t>Uudelleenkirjoitettu osia pakkausalgoritmista joka korjaa eilisen bugin. Nyt sekä pakkaus että purku toimii 100%. Hajautustaulukko kirjoitettu (iteraattorit avaimille ja arvoille puuttuu).</t>
+  </si>
+  <si>
+    <t>Hajautustaulukon iteraattorit toteutettu ja testattu.
+Kirjoitettu  yksikkötesti pääluokalle. Testattu erikokoisilla syötteillä,  käytetty testidata lisätty myös GitHubiin. JavaDoceja viimeistelty. Jäljellä työssä  prioriteettijonon toteutus.</t>
   </si>
 </sst>
 </file>
@@ -504,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,26 +647,38 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>41225</v>
       </c>
       <c r="B15" s="3">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
+    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>41226</v>
+      </c>
+      <c r="B16" s="3">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>41227</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -697,7 +716,7 @@
       </c>
       <c r="B24" s="9">
         <f>SUM(B6:B23)</f>
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C24" s="8"/>
     </row>

</xml_diff>